<commit_message>
Got the bleadvert.sb program to properly create a service
</commit_message>
<xml_diff>
--- a/docs/bl600TestMatrix.xlsx
+++ b/docs/bl600TestMatrix.xlsx
@@ -526,7 +526,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>